<commit_message>
xlsx_driver added to main, error handling, tests
</commit_message>
<xml_diff>
--- a/CalibrationData.xlsx
+++ b/CalibrationData.xlsx
@@ -634,7 +634,7 @@
   <dimension ref="B1:F40"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E45" activeCellId="0" sqref="E45"/>
+      <selection pane="topLeft" activeCell="F23" activeCellId="0" sqref="F23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -927,7 +927,7 @@
         <v>38</v>
       </c>
       <c r="C20" s="0" t="n">
-        <v>110</v>
+        <v>113</v>
       </c>
       <c r="D20" s="2" t="s">
         <v>10</v>
@@ -1170,7 +1170,7 @@
   <dimension ref="A1:A23"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E32" activeCellId="0" sqref="E32"/>
+      <selection pane="topLeft" activeCell="B21" activeCellId="0" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1256,7 +1256,7 @@
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="n">
         <f aca="false">Parameters!C20</f>
-        <v>110</v>
+        <v>113</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>